<commit_message>
Added quality report template and Test Survey template
</commit_message>
<xml_diff>
--- a/kimba-test-survey.xlsx
+++ b/kimba-test-survey.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\kimba-2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372FD01A-D992-48A0-9455-20D278186C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +24,563 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Local Setup</t>
+  </si>
+  <si>
+    <t>TC-001</t>
+  </si>
+  <si>
+    <t>TC-002</t>
+  </si>
+  <si>
+    <t>UAC Influence on Installation</t>
+  </si>
+  <si>
+    <t>TC-003</t>
+  </si>
+  <si>
+    <t>Turn UAC on and try to start the wizard.</t>
+  </si>
+  <si>
+    <t>The wizard should launch without issues.</t>
+  </si>
+  <si>
+    <t>TC-004</t>
+  </si>
+  <si>
+    <t>Turn UAC off and start the wizard.</t>
+  </si>
+  <si>
+    <t>The wizard should launch without influence from UAC.</t>
+  </si>
+  <si>
+    <t>Permission Restrictions</t>
+  </si>
+  <si>
+    <t>TC-005</t>
+  </si>
+  <si>
+    <t>Log in as a regular user and try launching the installer.</t>
+  </si>
+  <si>
+    <t>A warning message should appear if permission is restricted.</t>
+  </si>
+  <si>
+    <t>TC-006</t>
+  </si>
+  <si>
+    <t>Log in as an administrator and try launching the installer.</t>
+  </si>
+  <si>
+    <t>The installation should proceed without issues.</t>
+  </si>
+  <si>
+    <t>Pre-requisites Verification</t>
+  </si>
+  <si>
+    <t>TC-007</t>
+  </si>
+  <si>
+    <t>Launch the installer when pre-requisites (e.g., .NET, Java) are not installed.</t>
+  </si>
+  <si>
+    <r>
+      <t>.exe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> installer should download and install pre-requisites; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.msi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should open a download page.</t>
+    </r>
+  </si>
+  <si>
+    <t>TC-008</t>
+  </si>
+  <si>
+    <t>Verify that pre-requisite installation is skipped if they are already installed.</t>
+  </si>
+  <si>
+    <t>Installer should proceed without re-installing them.</t>
+  </si>
+  <si>
+    <t>Installation Process Management</t>
+  </si>
+  <si>
+    <t>TC-009</t>
+  </si>
+  <si>
+    <t>Try to start a second installation process while one is already running.</t>
+  </si>
+  <si>
+    <t>A warning message should prevent multiple instances.</t>
+  </si>
+  <si>
+    <t>Installation Types</t>
+  </si>
+  <si>
+    <t>TC-010</t>
+  </si>
+  <si>
+    <t>Perform a typical installation.</t>
+  </si>
+  <si>
+    <t>Installation should complete successfully.</t>
+  </si>
+  <si>
+    <t>TC-011</t>
+  </si>
+  <si>
+    <t>Perform a custom installation and deselect all elements.</t>
+  </si>
+  <si>
+    <t>The "OK" button should be disabled or prevent deselecting all elements.</t>
+  </si>
+  <si>
+    <t>TC-012</t>
+  </si>
+  <si>
+    <t>Perform a complete installation.</t>
+  </si>
+  <si>
+    <t>All components should install as expected.</t>
+  </si>
+  <si>
+    <t>Licensing Verification</t>
+  </si>
+  <si>
+    <t>TC-013</t>
+  </si>
+  <si>
+    <t>Verify that the licensing agreement meets user expectations and is printable.</t>
+  </si>
+  <si>
+    <t>The agreement should be clear and printable.</t>
+  </si>
+  <si>
+    <t>TC-014</t>
+  </si>
+  <si>
+    <t>Verify that the licensing mechanism cannot be bypassed.</t>
+  </si>
+  <si>
+    <t>Bypassing the license check should not be possible.</t>
+  </si>
+  <si>
+    <t>Disk Space &amp; Directory Selection</t>
+  </si>
+  <si>
+    <t>TC-015</t>
+  </si>
+  <si>
+    <t>Install on a system with insufficient disk space.</t>
+  </si>
+  <si>
+    <t>A warning should be displayed.</t>
+  </si>
+  <si>
+    <t>TC-016</t>
+  </si>
+  <si>
+    <t>Verify removable devices and mapped drives detection.</t>
+  </si>
+  <si>
+    <t>Installer should detect and show proper information.</t>
+  </si>
+  <si>
+    <t>TC-017</t>
+  </si>
+  <si>
+    <t>Install to the default folder.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Installation should proceed to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>%ProgramFiles%/%AppName%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>TC-018</t>
+  </si>
+  <si>
+    <t>Install to a custom directory (local, mapped, network, removable).</t>
+  </si>
+  <si>
+    <t>Installation should proceed if valid.</t>
+  </si>
+  <si>
+    <t>TC-019</t>
+  </si>
+  <si>
+    <t>Choose a folder with an unsupported file system (e.g., FAT32 for &gt;4GB files).</t>
+  </si>
+  <si>
+    <t>Installer should warn and prevent selection.</t>
+  </si>
+  <si>
+    <t>TC-020</t>
+  </si>
+  <si>
+    <t>Verify non-existing installation path creation.</t>
+  </si>
+  <si>
+    <t>Installer should create the path if it doesn't exist.</t>
+  </si>
+  <si>
+    <t>Reboot Scenarios</t>
+  </si>
+  <si>
+    <t>TC-021</t>
+  </si>
+  <si>
+    <t>Verify that installation resumes after a restart.</t>
+  </si>
+  <si>
+    <t>Installation should continue from the last step.</t>
+  </si>
+  <si>
+    <t>TC-022</t>
+  </si>
+  <si>
+    <t>Reboot unexpectedly during installation.</t>
+  </si>
+  <si>
+    <t>OS should load without failures or BSODs.</t>
+  </si>
+  <si>
+    <t>TC-023</t>
+  </si>
+  <si>
+    <t>Enter hibernate/standby during installation.</t>
+  </si>
+  <si>
+    <t>Installation should resume normally after waking up.</t>
+  </si>
+  <si>
+    <t>TC-024</t>
+  </si>
+  <si>
+    <t>Verify reboot prompt and user choice.</t>
+  </si>
+  <si>
+    <t>User should be prompted to reboot now or later.</t>
+  </si>
+  <si>
+    <t>GUI &amp; Usability</t>
+  </si>
+  <si>
+    <t>TC-025</t>
+  </si>
+  <si>
+    <t>Verify correct labels, logos, element positions, and navigation.</t>
+  </si>
+  <si>
+    <t>Everything should be aligned and readable.</t>
+  </si>
+  <si>
+    <t>TC-026</t>
+  </si>
+  <si>
+    <t>Verify installation help clarity.</t>
+  </si>
+  <si>
+    <t>Help should be clear and easy to follow.</t>
+  </si>
+  <si>
+    <t>TC-027</t>
+  </si>
+  <si>
+    <t>Attempt to proceed to the next step without completing the current step.</t>
+  </si>
+  <si>
+    <t>Should not be possible.</t>
+  </si>
+  <si>
+    <t>TC-028</t>
+  </si>
+  <si>
+    <t>Abort installation mid-way.</t>
+  </si>
+  <si>
+    <t>OS should not be damaged.</t>
+  </si>
+  <si>
+    <t>TC-029</t>
+  </si>
+  <si>
+    <t>Verify rollback after aborting.</t>
+  </si>
+  <si>
+    <t>All installed files should be removed.</t>
+  </si>
+  <si>
+    <t>Setup from Distribution Media (CD-ROM)</t>
+  </si>
+  <si>
+    <t>TC-030</t>
+  </si>
+  <si>
+    <t>Insert the installation CD and check autorun.</t>
+  </si>
+  <si>
+    <t>Installation should start automatically.</t>
+  </si>
+  <si>
+    <t>Network &amp; Internet Installation</t>
+  </si>
+  <si>
+    <t>TC-031</t>
+  </si>
+  <si>
+    <t>Install from a remote source.</t>
+  </si>
+  <si>
+    <t>Should install without issues.</t>
+  </si>
+  <si>
+    <t>TC-032</t>
+  </si>
+  <si>
+    <t>Install to a remote directory.</t>
+  </si>
+  <si>
+    <t>Should work per specifications.</t>
+  </si>
+  <si>
+    <t>TC-033</t>
+  </si>
+  <si>
+    <t>Verify permissions for non-shared folders or read-only directories.</t>
+  </si>
+  <si>
+    <t>Installation should be blocked with a warning.</t>
+  </si>
+  <si>
+    <t>TC-034</t>
+  </si>
+  <si>
+    <t>Resume installation after connection loss.</t>
+  </si>
+  <si>
+    <t>Download should continue from where it stopped.</t>
+  </si>
+  <si>
+    <t>Installation Result Validation</t>
+  </si>
+  <si>
+    <t>TC-035</t>
+  </si>
+  <si>
+    <t>Verify that necessary directories and shortcuts are created.</t>
+  </si>
+  <si>
+    <t>Directories and shortcuts should exist.</t>
+  </si>
+  <si>
+    <t>TC-036</t>
+  </si>
+  <si>
+    <t>Verify that installed components match user selections.</t>
+  </si>
+  <si>
+    <t>Installed files should match selections.</t>
+  </si>
+  <si>
+    <t>TC-037</t>
+  </si>
+  <si>
+    <t>Check Add/Remove Programs entry.</t>
+  </si>
+  <si>
+    <t>Entry should be present with correct version.</t>
+  </si>
+  <si>
+    <t>TC-038</t>
+  </si>
+  <si>
+    <t>Verify necessary system changes (e.g., services, registry).</t>
+  </si>
+  <si>
+    <t>Changes should be applied correctly.</t>
+  </si>
+  <si>
+    <t>Multi-User Support</t>
+  </si>
+  <si>
+    <t>TC-039</t>
+  </si>
+  <si>
+    <t>Verify shared settings for all system users.</t>
+  </si>
+  <si>
+    <t>Settings should be consistent.</t>
+  </si>
+  <si>
+    <t>TC-040</t>
+  </si>
+  <si>
+    <t>Verify personal settings for each user.</t>
+  </si>
+  <si>
+    <t>Each user should have separate settings.</t>
+  </si>
+  <si>
+    <t>Upgrade &amp; Update Scenarios</t>
+  </si>
+  <si>
+    <t>TC-041</t>
+  </si>
+  <si>
+    <t>Try installing a newer version over an old one.</t>
+  </si>
+  <si>
+    <t>Should display a warning or upgrade smoothly.</t>
+  </si>
+  <si>
+    <t>TC-042</t>
+  </si>
+  <si>
+    <t>Install an older version over a newer one.</t>
+  </si>
+  <si>
+    <t>Should not be allowed or require removal first.</t>
+  </si>
+  <si>
+    <t>TC-043</t>
+  </si>
+  <si>
+    <t>Verify that no duplicate directories are created.</t>
+  </si>
+  <si>
+    <t>Only one version should exist.</t>
+  </si>
+  <si>
+    <t>TC-044</t>
+  </si>
+  <si>
+    <t>Check if user data is retained post-upgrade.</t>
+  </si>
+  <si>
+    <t>Data should remain accessible.</t>
+  </si>
+  <si>
+    <t>Repair Option</t>
+  </si>
+  <si>
+    <t>TC-045</t>
+  </si>
+  <si>
+    <t>Access the Repair option from Add/Remove Programs.</t>
+  </si>
+  <si>
+    <t>Repair option should be available.</t>
+  </si>
+  <si>
+    <t>TC-046</t>
+  </si>
+  <si>
+    <t>Verify repair functionality (files, registry, shortcuts).</t>
+  </si>
+  <si>
+    <t>Repair should restore missing/corrupt files.</t>
+  </si>
+  <si>
+    <t>Smoke Test</t>
+  </si>
+  <si>
+    <t>TC-047</t>
+  </si>
+  <si>
+    <t>Verify the application launches correctly after installation.</t>
+  </si>
+  <si>
+    <t>The app should start without errors.</t>
+  </si>
+  <si>
+    <t>TC-048</t>
+  </si>
+  <si>
+    <t>Verify that all major functions work correctly post-installation.</t>
+  </si>
+  <si>
+    <t>The app should function properly.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +591,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +599,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +911,664 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="47.21875" customWidth="1"/>
+    <col min="2" max="2" width="66.21875" customWidth="1"/>
+    <col min="3" max="3" width="85.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>